<commit_message>
Estructura de Carpetas ADSO
</commit_message>
<xml_diff>
--- a/00_ruta/adso_cronograma_228118_V1.xlsx
+++ b/00_ruta/adso_cronograma_228118_V1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D88922A-F8A1-4501-95A6-80497BA4CFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6994B511-5C27-4513-80E5-335DE7724486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{2EF96F3D-4256-48DD-8CAA-143A5EBF2E06}"/>
   </bookViews>
@@ -3528,13 +3528,6 @@
 validar los requisitos con el cliente</t>
   </si>
   <si>
-    <t>Diagrama de casos de uso
-Diagrama de actividades
-Casos de uso extendido
-Modelo de dominio del Sistema
-Modelo Entidad Relación</t>
-  </si>
-  <si>
     <t>Ficha Técnica</t>
   </si>
   <si>
@@ -3627,6 +3620,13 @@
   <si>
     <t>Servidor de Aplicaciones Web
 Desarrollar Software: Web y Móvil</t>
+  </si>
+  <si>
+    <t>Modelo de dominio del Sistema
+Diagrama de casos de uso
+Diagrama de actividades
+Casos de uso extendido
+Modelo Entidad Relación</t>
   </si>
 </sst>
 </file>
@@ -5822,24 +5822,61 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -5849,7 +5886,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5860,83 +5896,23 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="42" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="43" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="85" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="52" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5946,16 +5922,40 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="83" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="21" fillId="0" borderId="41" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="42" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="43" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="44" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="85" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="83" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -5970,14 +5970,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
+          <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF0070C0"/>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6829,91 +6829,91 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="214"/>
-      <c r="C2" s="214"/>
-      <c r="D2" s="214"/>
-      <c r="E2" s="214"/>
-      <c r="F2" s="214"/>
+      <c r="B2" s="200"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="200"/>
+      <c r="F2" s="200"/>
     </row>
     <row r="3" spans="2:6" ht="30">
-      <c r="B3" s="212" t="s">
+      <c r="B3" s="198" t="s">
         <v>1131</v>
       </c>
-      <c r="C3" s="212"/>
-      <c r="D3" s="212"/>
-      <c r="E3" s="212"/>
-      <c r="F3" s="212"/>
+      <c r="C3" s="198"/>
+      <c r="D3" s="198"/>
+      <c r="E3" s="198"/>
+      <c r="F3" s="198"/>
     </row>
     <row r="4" spans="2:6" ht="30">
-      <c r="B4" s="212" t="s">
+      <c r="B4" s="198" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="212"/>
-      <c r="D4" s="212"/>
-      <c r="E4" s="212"/>
-      <c r="F4" s="212"/>
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="198"/>
+      <c r="F4" s="198"/>
     </row>
     <row r="5" spans="2:6" ht="17.25" thickBot="1">
-      <c r="B5" s="213"/>
-      <c r="C5" s="213"/>
-      <c r="D5" s="213"/>
-      <c r="E5" s="213"/>
-      <c r="F5" s="213"/>
+      <c r="B5" s="199"/>
+      <c r="C5" s="199"/>
+      <c r="D5" s="199"/>
+      <c r="E5" s="199"/>
+      <c r="F5" s="199"/>
     </row>
     <row r="6" spans="2:6" ht="17.25" thickTop="1">
       <c r="F6" s="3"/>
     </row>
     <row r="8" spans="2:6" ht="30">
-      <c r="B8" s="200" t="s">
+      <c r="B8" s="227" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="200"/>
-      <c r="D8" s="200"/>
-      <c r="E8" s="200"/>
-      <c r="F8" s="200"/>
+      <c r="C8" s="227"/>
+      <c r="D8" s="227"/>
+      <c r="E8" s="227"/>
+      <c r="F8" s="227"/>
     </row>
     <row r="10" spans="2:6" ht="17.25" thickBot="1"/>
     <row r="11" spans="2:6" ht="18.75" thickTop="1">
       <c r="B11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="221" t="s">
+      <c r="C11" s="208" t="s">
         <v>1128</v>
       </c>
-      <c r="D11" s="222"/>
-      <c r="E11" s="222"/>
-      <c r="F11" s="223"/>
+      <c r="D11" s="209"/>
+      <c r="E11" s="209"/>
+      <c r="F11" s="210"/>
     </row>
     <row r="12" spans="2:6" ht="18">
       <c r="B12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="198" t="s">
+      <c r="C12" s="211" t="s">
         <v>1132</v>
       </c>
-      <c r="D12" s="224"/>
-      <c r="E12" s="224"/>
-      <c r="F12" s="225"/>
+      <c r="D12" s="212"/>
+      <c r="E12" s="212"/>
+      <c r="F12" s="213"/>
     </row>
     <row r="13" spans="2:6" ht="18.75" thickBot="1">
       <c r="B13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="198" t="s">
+      <c r="C13" s="211" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="224"/>
-      <c r="E13" s="226"/>
-      <c r="F13" s="225"/>
+      <c r="D13" s="212"/>
+      <c r="E13" s="214"/>
+      <c r="F13" s="213"/>
     </row>
     <row r="14" spans="2:6" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="B14" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="198" t="s">
+      <c r="C14" s="211" t="s">
         <v>1133</v>
       </c>
-      <c r="D14" s="199"/>
+      <c r="D14" s="226"/>
       <c r="E14" s="28" t="s">
         <v>7</v>
       </c>
@@ -6925,10 +6925,10 @@
       <c r="B15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="227" t="s">
+      <c r="C15" s="215" t="s">
         <v>1129</v>
       </c>
-      <c r="D15" s="228"/>
+      <c r="D15" s="216"/>
       <c r="E15" s="29" t="s">
         <v>9</v>
       </c>
@@ -6940,10 +6940,10 @@
       <c r="B16" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="229" t="s">
+      <c r="C16" s="217" t="s">
         <v>1133</v>
       </c>
-      <c r="D16" s="230"/>
+      <c r="D16" s="218"/>
       <c r="E16" s="30" t="s">
         <v>10</v>
       </c>
@@ -6953,8 +6953,8 @@
     </row>
     <row r="17" spans="2:16" ht="17.25" thickTop="1">
       <c r="B17" s="4"/>
-      <c r="C17" s="218"/>
-      <c r="D17" s="218"/>
+      <c r="C17" s="204"/>
+      <c r="D17" s="204"/>
     </row>
     <row r="18" spans="2:16" ht="19.899999999999999" customHeight="1"/>
     <row r="19" spans="2:16" ht="19.899999999999999" customHeight="1">
@@ -6973,10 +6973,10 @@
       <c r="C21" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="219" t="s">
+      <c r="D21" s="205" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="219"/>
+      <c r="E21" s="205"/>
       <c r="F21" s="17" t="s">
         <v>16</v>
       </c>
@@ -6988,10 +6988,10 @@
       <c r="C22" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="220" t="s">
+      <c r="D22" s="206" t="s">
         <v>1133</v>
       </c>
-      <c r="E22" s="220"/>
+      <c r="E22" s="206"/>
       <c r="F22" s="20" t="s">
         <v>1130</v>
       </c>
@@ -7048,8 +7048,8 @@
     <row r="30" spans="2:16" ht="25.5" customHeight="1" thickBot="1">
       <c r="B30" s="24"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="208"/>
-      <c r="E30" s="208"/>
+      <c r="D30" s="222"/>
+      <c r="E30" s="222"/>
       <c r="F30" s="26"/>
     </row>
     <row r="31" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1"/>
@@ -7060,53 +7060,53 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B34" s="209" t="s">
+      <c r="B34" s="223" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="210"/>
-      <c r="D34" s="210"/>
-      <c r="E34" s="210"/>
-      <c r="F34" s="211"/>
+      <c r="C34" s="224"/>
+      <c r="D34" s="224"/>
+      <c r="E34" s="224"/>
+      <c r="F34" s="225"/>
     </row>
     <row r="35" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B35" s="215" t="s">
+      <c r="B35" s="201" t="s">
         <v>1133</v>
       </c>
-      <c r="C35" s="216"/>
-      <c r="D35" s="216"/>
-      <c r="E35" s="216"/>
-      <c r="F35" s="217"/>
+      <c r="C35" s="202"/>
+      <c r="D35" s="202"/>
+      <c r="E35" s="202"/>
+      <c r="F35" s="203"/>
     </row>
     <row r="36" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B36" s="201"/>
-      <c r="C36" s="202"/>
-      <c r="D36" s="202"/>
-      <c r="E36" s="202"/>
-      <c r="F36" s="203"/>
+      <c r="B36" s="228"/>
+      <c r="C36" s="229"/>
+      <c r="D36" s="229"/>
+      <c r="E36" s="229"/>
+      <c r="F36" s="230"/>
       <c r="J36" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B37" s="201"/>
-      <c r="C37" s="202"/>
-      <c r="D37" s="202"/>
-      <c r="E37" s="202"/>
-      <c r="F37" s="203"/>
+      <c r="B37" s="228"/>
+      <c r="C37" s="229"/>
+      <c r="D37" s="229"/>
+      <c r="E37" s="229"/>
+      <c r="F37" s="230"/>
     </row>
     <row r="38" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B38" s="201"/>
-      <c r="C38" s="202"/>
-      <c r="D38" s="202"/>
-      <c r="E38" s="202"/>
-      <c r="F38" s="203"/>
+      <c r="B38" s="228"/>
+      <c r="C38" s="229"/>
+      <c r="D38" s="229"/>
+      <c r="E38" s="229"/>
+      <c r="F38" s="230"/>
     </row>
     <row r="39" spans="1:13" s="7" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B39" s="204"/>
-      <c r="C39" s="205"/>
-      <c r="D39" s="205"/>
-      <c r="E39" s="205"/>
-      <c r="F39" s="206"/>
+      <c r="B39" s="219"/>
+      <c r="C39" s="220"/>
+      <c r="D39" s="220"/>
+      <c r="E39" s="220"/>
+      <c r="F39" s="221"/>
     </row>
     <row r="40" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A40" s="7"/>
@@ -7267,6 +7267,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B34:F34"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
@@ -7283,18 +7295,6 @@
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -15802,8 +15802,8 @@
   <dimension ref="A1:BR60"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="11" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -15825,296 +15825,296 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:70" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="231"/>
-      <c r="B1" s="231"/>
-      <c r="C1" s="231"/>
-      <c r="D1" s="231"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="231"/>
-      <c r="G1" s="231"/>
-      <c r="H1" s="231"/>
-      <c r="I1" s="231"/>
-      <c r="J1" s="231"/>
-      <c r="K1" s="231"/>
-      <c r="L1" s="231"/>
-      <c r="M1" s="231"/>
-      <c r="N1" s="231"/>
-      <c r="O1" s="231"/>
-      <c r="P1" s="231"/>
-      <c r="Q1" s="231"/>
-      <c r="R1" s="231"/>
-      <c r="S1" s="231"/>
-      <c r="T1" s="231"/>
-      <c r="U1" s="231"/>
-      <c r="V1" s="231"/>
-      <c r="W1" s="231"/>
-      <c r="X1" s="231"/>
-      <c r="Y1" s="231"/>
-      <c r="Z1" s="231"/>
-      <c r="AA1" s="231"/>
-      <c r="AB1" s="231"/>
-      <c r="AC1" s="231"/>
-      <c r="AD1" s="231"/>
-      <c r="AE1" s="231"/>
-      <c r="AF1" s="231"/>
-      <c r="AG1" s="231"/>
-      <c r="AH1" s="231"/>
-      <c r="AI1" s="231"/>
-      <c r="AJ1" s="231"/>
-      <c r="AK1" s="231"/>
-      <c r="AL1" s="231"/>
-      <c r="AM1" s="231"/>
-      <c r="AN1" s="231"/>
-      <c r="AO1" s="231"/>
-      <c r="AP1" s="231"/>
-      <c r="AQ1" s="231"/>
-      <c r="AR1" s="231"/>
-      <c r="AS1" s="231"/>
-      <c r="AT1" s="231"/>
-      <c r="AU1" s="231"/>
-      <c r="AV1" s="231"/>
-      <c r="AW1" s="231"/>
-      <c r="AX1" s="231"/>
-      <c r="AY1" s="231"/>
-      <c r="AZ1" s="231"/>
-      <c r="BA1" s="231"/>
-      <c r="BB1" s="231"/>
-      <c r="BC1" s="231"/>
-      <c r="BD1" s="231"/>
-      <c r="BE1" s="231"/>
-      <c r="BF1" s="231"/>
-      <c r="BG1" s="231"/>
-      <c r="BH1" s="231"/>
-      <c r="BI1" s="231"/>
-      <c r="BJ1" s="231"/>
-      <c r="BK1" s="231"/>
-      <c r="BL1" s="231"/>
-      <c r="BM1" s="231"/>
-      <c r="BN1" s="231"/>
-      <c r="BO1" s="231"/>
-      <c r="BP1" s="231"/>
-      <c r="BQ1" s="231"/>
-      <c r="BR1" s="231"/>
+      <c r="A1" s="236"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
+      <c r="K1" s="236"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
+      <c r="N1" s="236"/>
+      <c r="O1" s="236"/>
+      <c r="P1" s="236"/>
+      <c r="Q1" s="236"/>
+      <c r="R1" s="236"/>
+      <c r="S1" s="236"/>
+      <c r="T1" s="236"/>
+      <c r="U1" s="236"/>
+      <c r="V1" s="236"/>
+      <c r="W1" s="236"/>
+      <c r="X1" s="236"/>
+      <c r="Y1" s="236"/>
+      <c r="Z1" s="236"/>
+      <c r="AA1" s="236"/>
+      <c r="AB1" s="236"/>
+      <c r="AC1" s="236"/>
+      <c r="AD1" s="236"/>
+      <c r="AE1" s="236"/>
+      <c r="AF1" s="236"/>
+      <c r="AG1" s="236"/>
+      <c r="AH1" s="236"/>
+      <c r="AI1" s="236"/>
+      <c r="AJ1" s="236"/>
+      <c r="AK1" s="236"/>
+      <c r="AL1" s="236"/>
+      <c r="AM1" s="236"/>
+      <c r="AN1" s="236"/>
+      <c r="AO1" s="236"/>
+      <c r="AP1" s="236"/>
+      <c r="AQ1" s="236"/>
+      <c r="AR1" s="236"/>
+      <c r="AS1" s="236"/>
+      <c r="AT1" s="236"/>
+      <c r="AU1" s="236"/>
+      <c r="AV1" s="236"/>
+      <c r="AW1" s="236"/>
+      <c r="AX1" s="236"/>
+      <c r="AY1" s="236"/>
+      <c r="AZ1" s="236"/>
+      <c r="BA1" s="236"/>
+      <c r="BB1" s="236"/>
+      <c r="BC1" s="236"/>
+      <c r="BD1" s="236"/>
+      <c r="BE1" s="236"/>
+      <c r="BF1" s="236"/>
+      <c r="BG1" s="236"/>
+      <c r="BH1" s="236"/>
+      <c r="BI1" s="236"/>
+      <c r="BJ1" s="236"/>
+      <c r="BK1" s="236"/>
+      <c r="BL1" s="236"/>
+      <c r="BM1" s="236"/>
+      <c r="BN1" s="236"/>
+      <c r="BO1" s="236"/>
+      <c r="BP1" s="236"/>
+      <c r="BQ1" s="236"/>
+      <c r="BR1" s="236"/>
     </row>
     <row r="2" spans="1:70" s="46" customFormat="1" ht="20.25">
-      <c r="A2" s="232" t="s">
+      <c r="A2" s="237" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="232"/>
-      <c r="C2" s="232"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
-      <c r="G2" s="232"/>
-      <c r="H2" s="231"/>
-      <c r="I2" s="232"/>
-      <c r="J2" s="232"/>
-      <c r="K2" s="232"/>
-      <c r="L2" s="232"/>
-      <c r="M2" s="232"/>
-      <c r="N2" s="232"/>
-      <c r="O2" s="232"/>
-      <c r="P2" s="232"/>
-      <c r="Q2" s="232"/>
-      <c r="R2" s="232"/>
-      <c r="S2" s="232"/>
-      <c r="T2" s="232"/>
-      <c r="U2" s="232"/>
-      <c r="V2" s="232"/>
-      <c r="W2" s="232"/>
-      <c r="X2" s="232"/>
-      <c r="Y2" s="232"/>
-      <c r="Z2" s="232"/>
-      <c r="AA2" s="232"/>
-      <c r="AB2" s="232"/>
-      <c r="AC2" s="232"/>
-      <c r="AD2" s="232"/>
-      <c r="AE2" s="232"/>
-      <c r="AF2" s="232"/>
-      <c r="AG2" s="232"/>
-      <c r="AH2" s="232"/>
-      <c r="AI2" s="232"/>
-      <c r="AJ2" s="232"/>
-      <c r="AK2" s="232"/>
-      <c r="AL2" s="232"/>
-      <c r="AM2" s="232"/>
-      <c r="AN2" s="232"/>
-      <c r="AO2" s="232"/>
-      <c r="AP2" s="232"/>
-      <c r="AQ2" s="232"/>
-      <c r="AR2" s="232"/>
-      <c r="AS2" s="232"/>
-      <c r="AT2" s="232"/>
-      <c r="AU2" s="232"/>
-      <c r="AV2" s="232"/>
-      <c r="AW2" s="232"/>
-      <c r="AX2" s="232"/>
-      <c r="AY2" s="232"/>
-      <c r="AZ2" s="232"/>
-      <c r="BA2" s="232"/>
-      <c r="BB2" s="232"/>
-      <c r="BC2" s="232"/>
-      <c r="BD2" s="232"/>
-      <c r="BE2" s="232"/>
-      <c r="BF2" s="232"/>
-      <c r="BG2" s="232"/>
-      <c r="BH2" s="232"/>
-      <c r="BI2" s="232"/>
-      <c r="BJ2" s="232"/>
-      <c r="BK2" s="232"/>
-      <c r="BL2" s="232"/>
-      <c r="BM2" s="232"/>
-      <c r="BN2" s="232"/>
-      <c r="BO2" s="232"/>
-      <c r="BP2" s="232"/>
-      <c r="BQ2" s="232"/>
-      <c r="BR2" s="233"/>
+      <c r="B2" s="237"/>
+      <c r="C2" s="237"/>
+      <c r="D2" s="237"/>
+      <c r="E2" s="237"/>
+      <c r="F2" s="237"/>
+      <c r="G2" s="237"/>
+      <c r="H2" s="236"/>
+      <c r="I2" s="237"/>
+      <c r="J2" s="237"/>
+      <c r="K2" s="237"/>
+      <c r="L2" s="237"/>
+      <c r="M2" s="237"/>
+      <c r="N2" s="237"/>
+      <c r="O2" s="237"/>
+      <c r="P2" s="237"/>
+      <c r="Q2" s="237"/>
+      <c r="R2" s="237"/>
+      <c r="S2" s="237"/>
+      <c r="T2" s="237"/>
+      <c r="U2" s="237"/>
+      <c r="V2" s="237"/>
+      <c r="W2" s="237"/>
+      <c r="X2" s="237"/>
+      <c r="Y2" s="237"/>
+      <c r="Z2" s="237"/>
+      <c r="AA2" s="237"/>
+      <c r="AB2" s="237"/>
+      <c r="AC2" s="237"/>
+      <c r="AD2" s="237"/>
+      <c r="AE2" s="237"/>
+      <c r="AF2" s="237"/>
+      <c r="AG2" s="237"/>
+      <c r="AH2" s="237"/>
+      <c r="AI2" s="237"/>
+      <c r="AJ2" s="237"/>
+      <c r="AK2" s="237"/>
+      <c r="AL2" s="237"/>
+      <c r="AM2" s="237"/>
+      <c r="AN2" s="237"/>
+      <c r="AO2" s="237"/>
+      <c r="AP2" s="237"/>
+      <c r="AQ2" s="237"/>
+      <c r="AR2" s="237"/>
+      <c r="AS2" s="237"/>
+      <c r="AT2" s="237"/>
+      <c r="AU2" s="237"/>
+      <c r="AV2" s="237"/>
+      <c r="AW2" s="237"/>
+      <c r="AX2" s="237"/>
+      <c r="AY2" s="237"/>
+      <c r="AZ2" s="237"/>
+      <c r="BA2" s="237"/>
+      <c r="BB2" s="237"/>
+      <c r="BC2" s="237"/>
+      <c r="BD2" s="237"/>
+      <c r="BE2" s="237"/>
+      <c r="BF2" s="237"/>
+      <c r="BG2" s="237"/>
+      <c r="BH2" s="237"/>
+      <c r="BI2" s="237"/>
+      <c r="BJ2" s="237"/>
+      <c r="BK2" s="237"/>
+      <c r="BL2" s="237"/>
+      <c r="BM2" s="237"/>
+      <c r="BN2" s="237"/>
+      <c r="BO2" s="237"/>
+      <c r="BP2" s="237"/>
+      <c r="BQ2" s="237"/>
+      <c r="BR2" s="238"/>
     </row>
     <row r="3" spans="1:70" s="46" customFormat="1" ht="20.25">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="237" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="232"/>
-      <c r="C3" s="232"/>
-      <c r="D3" s="232"/>
-      <c r="E3" s="232"/>
-      <c r="F3" s="232"/>
-      <c r="G3" s="232"/>
-      <c r="H3" s="231"/>
-      <c r="I3" s="232"/>
-      <c r="J3" s="232"/>
-      <c r="K3" s="232"/>
-      <c r="L3" s="232"/>
-      <c r="M3" s="232"/>
-      <c r="N3" s="232"/>
-      <c r="O3" s="232"/>
-      <c r="P3" s="232"/>
-      <c r="Q3" s="232"/>
-      <c r="R3" s="232"/>
-      <c r="S3" s="232"/>
-      <c r="T3" s="232"/>
-      <c r="U3" s="232"/>
-      <c r="V3" s="232"/>
-      <c r="W3" s="232"/>
-      <c r="X3" s="232"/>
-      <c r="Y3" s="232"/>
-      <c r="Z3" s="232"/>
-      <c r="AA3" s="232"/>
-      <c r="AB3" s="232"/>
-      <c r="AC3" s="232"/>
-      <c r="AD3" s="232"/>
-      <c r="AE3" s="232"/>
-      <c r="AF3" s="232"/>
-      <c r="AG3" s="232"/>
-      <c r="AH3" s="232"/>
-      <c r="AI3" s="232"/>
-      <c r="AJ3" s="232"/>
-      <c r="AK3" s="232"/>
-      <c r="AL3" s="232"/>
-      <c r="AM3" s="232"/>
-      <c r="AN3" s="232"/>
-      <c r="AO3" s="232"/>
-      <c r="AP3" s="232"/>
-      <c r="AQ3" s="232"/>
-      <c r="AR3" s="232"/>
-      <c r="AS3" s="232"/>
-      <c r="AT3" s="232"/>
-      <c r="AU3" s="232"/>
-      <c r="AV3" s="232"/>
-      <c r="AW3" s="232"/>
-      <c r="AX3" s="232"/>
-      <c r="AY3" s="232"/>
-      <c r="AZ3" s="232"/>
-      <c r="BA3" s="232"/>
-      <c r="BB3" s="232"/>
-      <c r="BC3" s="232"/>
-      <c r="BD3" s="232"/>
-      <c r="BE3" s="232"/>
-      <c r="BF3" s="232"/>
-      <c r="BG3" s="232"/>
-      <c r="BH3" s="232"/>
-      <c r="BI3" s="232"/>
-      <c r="BJ3" s="232"/>
-      <c r="BK3" s="232"/>
-      <c r="BL3" s="232"/>
-      <c r="BM3" s="232"/>
-      <c r="BN3" s="232"/>
-      <c r="BO3" s="232"/>
-      <c r="BP3" s="232"/>
-      <c r="BQ3" s="232"/>
-      <c r="BR3" s="233"/>
+      <c r="B3" s="237"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="236"/>
+      <c r="I3" s="237"/>
+      <c r="J3" s="237"/>
+      <c r="K3" s="237"/>
+      <c r="L3" s="237"/>
+      <c r="M3" s="237"/>
+      <c r="N3" s="237"/>
+      <c r="O3" s="237"/>
+      <c r="P3" s="237"/>
+      <c r="Q3" s="237"/>
+      <c r="R3" s="237"/>
+      <c r="S3" s="237"/>
+      <c r="T3" s="237"/>
+      <c r="U3" s="237"/>
+      <c r="V3" s="237"/>
+      <c r="W3" s="237"/>
+      <c r="X3" s="237"/>
+      <c r="Y3" s="237"/>
+      <c r="Z3" s="237"/>
+      <c r="AA3" s="237"/>
+      <c r="AB3" s="237"/>
+      <c r="AC3" s="237"/>
+      <c r="AD3" s="237"/>
+      <c r="AE3" s="237"/>
+      <c r="AF3" s="237"/>
+      <c r="AG3" s="237"/>
+      <c r="AH3" s="237"/>
+      <c r="AI3" s="237"/>
+      <c r="AJ3" s="237"/>
+      <c r="AK3" s="237"/>
+      <c r="AL3" s="237"/>
+      <c r="AM3" s="237"/>
+      <c r="AN3" s="237"/>
+      <c r="AO3" s="237"/>
+      <c r="AP3" s="237"/>
+      <c r="AQ3" s="237"/>
+      <c r="AR3" s="237"/>
+      <c r="AS3" s="237"/>
+      <c r="AT3" s="237"/>
+      <c r="AU3" s="237"/>
+      <c r="AV3" s="237"/>
+      <c r="AW3" s="237"/>
+      <c r="AX3" s="237"/>
+      <c r="AY3" s="237"/>
+      <c r="AZ3" s="237"/>
+      <c r="BA3" s="237"/>
+      <c r="BB3" s="237"/>
+      <c r="BC3" s="237"/>
+      <c r="BD3" s="237"/>
+      <c r="BE3" s="237"/>
+      <c r="BF3" s="237"/>
+      <c r="BG3" s="237"/>
+      <c r="BH3" s="237"/>
+      <c r="BI3" s="237"/>
+      <c r="BJ3" s="237"/>
+      <c r="BK3" s="237"/>
+      <c r="BL3" s="237"/>
+      <c r="BM3" s="237"/>
+      <c r="BN3" s="237"/>
+      <c r="BO3" s="237"/>
+      <c r="BP3" s="237"/>
+      <c r="BQ3" s="237"/>
+      <c r="BR3" s="238"/>
     </row>
     <row r="4" spans="1:70" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A4" s="234"/>
-      <c r="B4" s="234"/>
-      <c r="C4" s="234"/>
-      <c r="D4" s="234"/>
-      <c r="E4" s="234"/>
-      <c r="F4" s="234"/>
-      <c r="G4" s="234"/>
-      <c r="H4" s="234"/>
-      <c r="I4" s="234"/>
-      <c r="J4" s="234"/>
-      <c r="K4" s="234"/>
-      <c r="L4" s="234"/>
-      <c r="M4" s="234"/>
-      <c r="N4" s="234"/>
-      <c r="O4" s="234"/>
-      <c r="P4" s="234"/>
-      <c r="Q4" s="234"/>
-      <c r="R4" s="234"/>
-      <c r="S4" s="234"/>
-      <c r="T4" s="234"/>
-      <c r="U4" s="234"/>
-      <c r="V4" s="234"/>
-      <c r="W4" s="234"/>
-      <c r="X4" s="234"/>
-      <c r="Y4" s="234"/>
-      <c r="Z4" s="234"/>
-      <c r="AA4" s="234"/>
-      <c r="AB4" s="234"/>
-      <c r="AC4" s="234"/>
-      <c r="AD4" s="234"/>
-      <c r="AE4" s="234"/>
-      <c r="AF4" s="234"/>
-      <c r="AG4" s="234"/>
-      <c r="AH4" s="234"/>
-      <c r="AI4" s="234"/>
-      <c r="AJ4" s="234"/>
-      <c r="AK4" s="234"/>
-      <c r="AL4" s="234"/>
-      <c r="AM4" s="234"/>
-      <c r="AN4" s="234"/>
-      <c r="AO4" s="234"/>
-      <c r="AP4" s="234"/>
-      <c r="AQ4" s="234"/>
-      <c r="AR4" s="234"/>
-      <c r="AS4" s="234"/>
-      <c r="AT4" s="234"/>
-      <c r="AU4" s="234"/>
-      <c r="AV4" s="234"/>
-      <c r="AW4" s="234"/>
-      <c r="AX4" s="234"/>
-      <c r="AY4" s="234"/>
-      <c r="AZ4" s="234"/>
-      <c r="BA4" s="234"/>
-      <c r="BB4" s="234"/>
-      <c r="BC4" s="234"/>
-      <c r="BD4" s="234"/>
-      <c r="BE4" s="234"/>
-      <c r="BF4" s="234"/>
-      <c r="BG4" s="234"/>
-      <c r="BH4" s="234"/>
-      <c r="BI4" s="234"/>
-      <c r="BJ4" s="234"/>
-      <c r="BK4" s="234"/>
-      <c r="BL4" s="234"/>
-      <c r="BM4" s="234"/>
-      <c r="BN4" s="234"/>
-      <c r="BO4" s="234"/>
-      <c r="BP4" s="234"/>
-      <c r="BQ4" s="234"/>
-      <c r="BR4" s="235"/>
+      <c r="A4" s="239"/>
+      <c r="B4" s="239"/>
+      <c r="C4" s="239"/>
+      <c r="D4" s="239"/>
+      <c r="E4" s="239"/>
+      <c r="F4" s="239"/>
+      <c r="G4" s="239"/>
+      <c r="H4" s="239"/>
+      <c r="I4" s="239"/>
+      <c r="J4" s="239"/>
+      <c r="K4" s="239"/>
+      <c r="L4" s="239"/>
+      <c r="M4" s="239"/>
+      <c r="N4" s="239"/>
+      <c r="O4" s="239"/>
+      <c r="P4" s="239"/>
+      <c r="Q4" s="239"/>
+      <c r="R4" s="239"/>
+      <c r="S4" s="239"/>
+      <c r="T4" s="239"/>
+      <c r="U4" s="239"/>
+      <c r="V4" s="239"/>
+      <c r="W4" s="239"/>
+      <c r="X4" s="239"/>
+      <c r="Y4" s="239"/>
+      <c r="Z4" s="239"/>
+      <c r="AA4" s="239"/>
+      <c r="AB4" s="239"/>
+      <c r="AC4" s="239"/>
+      <c r="AD4" s="239"/>
+      <c r="AE4" s="239"/>
+      <c r="AF4" s="239"/>
+      <c r="AG4" s="239"/>
+      <c r="AH4" s="239"/>
+      <c r="AI4" s="239"/>
+      <c r="AJ4" s="239"/>
+      <c r="AK4" s="239"/>
+      <c r="AL4" s="239"/>
+      <c r="AM4" s="239"/>
+      <c r="AN4" s="239"/>
+      <c r="AO4" s="239"/>
+      <c r="AP4" s="239"/>
+      <c r="AQ4" s="239"/>
+      <c r="AR4" s="239"/>
+      <c r="AS4" s="239"/>
+      <c r="AT4" s="239"/>
+      <c r="AU4" s="239"/>
+      <c r="AV4" s="239"/>
+      <c r="AW4" s="239"/>
+      <c r="AX4" s="239"/>
+      <c r="AY4" s="239"/>
+      <c r="AZ4" s="239"/>
+      <c r="BA4" s="239"/>
+      <c r="BB4" s="239"/>
+      <c r="BC4" s="239"/>
+      <c r="BD4" s="239"/>
+      <c r="BE4" s="239"/>
+      <c r="BF4" s="239"/>
+      <c r="BG4" s="239"/>
+      <c r="BH4" s="239"/>
+      <c r="BI4" s="239"/>
+      <c r="BJ4" s="239"/>
+      <c r="BK4" s="239"/>
+      <c r="BL4" s="239"/>
+      <c r="BM4" s="239"/>
+      <c r="BN4" s="239"/>
+      <c r="BO4" s="239"/>
+      <c r="BP4" s="239"/>
+      <c r="BQ4" s="239"/>
+      <c r="BR4" s="240"/>
     </row>
     <row r="5" spans="1:70" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1" thickTop="1">
       <c r="A5" s="169"/>
@@ -16229,11 +16229,11 @@
         <v>26</v>
       </c>
       <c r="C8" s="182"/>
-      <c r="D8" s="245">
+      <c r="D8" s="235">
         <v>45040</v>
       </c>
-      <c r="E8" s="245"/>
-      <c r="F8" s="245"/>
+      <c r="E8" s="235"/>
+      <c r="F8" s="235"/>
       <c r="G8" s="42"/>
       <c r="H8" s="42"/>
       <c r="K8" s="196" t="s">
@@ -16242,179 +16242,179 @@
       <c r="L8" s="32">
         <v>1</v>
       </c>
-      <c r="O8" s="240" t="str">
+      <c r="O8" s="232" t="str">
         <f>"Semana "&amp;(O10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 1</v>
       </c>
-      <c r="P8" s="241"/>
-      <c r="Q8" s="241"/>
-      <c r="R8" s="241"/>
-      <c r="S8" s="241"/>
-      <c r="T8" s="241"/>
-      <c r="U8" s="242"/>
-      <c r="V8" s="240" t="str">
+      <c r="P8" s="233"/>
+      <c r="Q8" s="233"/>
+      <c r="R8" s="233"/>
+      <c r="S8" s="233"/>
+      <c r="T8" s="233"/>
+      <c r="U8" s="234"/>
+      <c r="V8" s="232" t="str">
         <f>"Semana "&amp;(V10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 2</v>
       </c>
-      <c r="W8" s="241"/>
-      <c r="X8" s="241"/>
-      <c r="Y8" s="241"/>
-      <c r="Z8" s="241"/>
-      <c r="AA8" s="241"/>
-      <c r="AB8" s="242"/>
-      <c r="AC8" s="240" t="str">
+      <c r="W8" s="233"/>
+      <c r="X8" s="233"/>
+      <c r="Y8" s="233"/>
+      <c r="Z8" s="233"/>
+      <c r="AA8" s="233"/>
+      <c r="AB8" s="234"/>
+      <c r="AC8" s="232" t="str">
         <f>"Semana "&amp;(AC10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 3</v>
       </c>
-      <c r="AD8" s="241"/>
-      <c r="AE8" s="241"/>
-      <c r="AF8" s="241"/>
-      <c r="AG8" s="241"/>
-      <c r="AH8" s="241"/>
-      <c r="AI8" s="242"/>
-      <c r="AJ8" s="240" t="str">
+      <c r="AD8" s="233"/>
+      <c r="AE8" s="233"/>
+      <c r="AF8" s="233"/>
+      <c r="AG8" s="233"/>
+      <c r="AH8" s="233"/>
+      <c r="AI8" s="234"/>
+      <c r="AJ8" s="232" t="str">
         <f>"Semana "&amp;(AJ10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 4</v>
       </c>
-      <c r="AK8" s="241"/>
-      <c r="AL8" s="241"/>
-      <c r="AM8" s="241"/>
-      <c r="AN8" s="241"/>
-      <c r="AO8" s="241"/>
-      <c r="AP8" s="242"/>
-      <c r="AQ8" s="240" t="str">
+      <c r="AK8" s="233"/>
+      <c r="AL8" s="233"/>
+      <c r="AM8" s="233"/>
+      <c r="AN8" s="233"/>
+      <c r="AO8" s="233"/>
+      <c r="AP8" s="234"/>
+      <c r="AQ8" s="232" t="str">
         <f>"Semana "&amp;(AQ10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 5</v>
       </c>
-      <c r="AR8" s="241"/>
-      <c r="AS8" s="241"/>
-      <c r="AT8" s="241"/>
-      <c r="AU8" s="241"/>
-      <c r="AV8" s="241"/>
-      <c r="AW8" s="242"/>
-      <c r="AX8" s="240" t="str">
+      <c r="AR8" s="233"/>
+      <c r="AS8" s="233"/>
+      <c r="AT8" s="233"/>
+      <c r="AU8" s="233"/>
+      <c r="AV8" s="233"/>
+      <c r="AW8" s="234"/>
+      <c r="AX8" s="232" t="str">
         <f>"Semana "&amp;(AX10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 6</v>
       </c>
-      <c r="AY8" s="241"/>
-      <c r="AZ8" s="241"/>
-      <c r="BA8" s="241"/>
-      <c r="BB8" s="241"/>
-      <c r="BC8" s="241"/>
-      <c r="BD8" s="242"/>
-      <c r="BE8" s="240" t="str">
+      <c r="AY8" s="233"/>
+      <c r="AZ8" s="233"/>
+      <c r="BA8" s="233"/>
+      <c r="BB8" s="233"/>
+      <c r="BC8" s="233"/>
+      <c r="BD8" s="234"/>
+      <c r="BE8" s="232" t="str">
         <f>"Semana "&amp;(BE10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 7</v>
       </c>
-      <c r="BF8" s="241"/>
-      <c r="BG8" s="241"/>
-      <c r="BH8" s="241"/>
-      <c r="BI8" s="241"/>
-      <c r="BJ8" s="241"/>
-      <c r="BK8" s="242"/>
-      <c r="BL8" s="240" t="str">
+      <c r="BF8" s="233"/>
+      <c r="BG8" s="233"/>
+      <c r="BH8" s="233"/>
+      <c r="BI8" s="233"/>
+      <c r="BJ8" s="233"/>
+      <c r="BK8" s="234"/>
+      <c r="BL8" s="232" t="str">
         <f>"Semana "&amp;(BL10-($D$8-WEEKDAY($D$8,1)+2))/7+1</f>
         <v>Semana 8</v>
       </c>
-      <c r="BM8" s="241"/>
-      <c r="BN8" s="241"/>
-      <c r="BO8" s="241"/>
-      <c r="BP8" s="241"/>
-      <c r="BQ8" s="241"/>
-      <c r="BR8" s="243"/>
+      <c r="BM8" s="233"/>
+      <c r="BN8" s="233"/>
+      <c r="BO8" s="233"/>
+      <c r="BP8" s="233"/>
+      <c r="BQ8" s="233"/>
+      <c r="BR8" s="245"/>
     </row>
     <row r="9" spans="1:70" ht="17.25" customHeight="1">
       <c r="B9" s="181" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="182"/>
-      <c r="D9" s="244" t="s">
+      <c r="D9" s="231" t="s">
         <v>1113</v>
       </c>
-      <c r="E9" s="244"/>
-      <c r="F9" s="244"/>
+      <c r="E9" s="231"/>
+      <c r="F9" s="231"/>
       <c r="G9" s="43"/>
       <c r="H9" s="43"/>
-      <c r="O9" s="236">
+      <c r="O9" s="241">
         <f>O10</f>
         <v>45040</v>
       </c>
-      <c r="P9" s="237"/>
-      <c r="Q9" s="237"/>
-      <c r="R9" s="237"/>
-      <c r="S9" s="237"/>
-      <c r="T9" s="237"/>
-      <c r="U9" s="238"/>
-      <c r="V9" s="236">
+      <c r="P9" s="242"/>
+      <c r="Q9" s="242"/>
+      <c r="R9" s="242"/>
+      <c r="S9" s="242"/>
+      <c r="T9" s="242"/>
+      <c r="U9" s="243"/>
+      <c r="V9" s="241">
         <f>V10</f>
         <v>45047</v>
       </c>
-      <c r="W9" s="237"/>
-      <c r="X9" s="237"/>
-      <c r="Y9" s="237"/>
-      <c r="Z9" s="237"/>
-      <c r="AA9" s="237"/>
-      <c r="AB9" s="238"/>
-      <c r="AC9" s="236">
+      <c r="W9" s="242"/>
+      <c r="X9" s="242"/>
+      <c r="Y9" s="242"/>
+      <c r="Z9" s="242"/>
+      <c r="AA9" s="242"/>
+      <c r="AB9" s="243"/>
+      <c r="AC9" s="241">
         <f>AC10</f>
         <v>45054</v>
       </c>
-      <c r="AD9" s="237"/>
-      <c r="AE9" s="237"/>
-      <c r="AF9" s="237"/>
-      <c r="AG9" s="237"/>
-      <c r="AH9" s="237"/>
-      <c r="AI9" s="238"/>
-      <c r="AJ9" s="236">
+      <c r="AD9" s="242"/>
+      <c r="AE9" s="242"/>
+      <c r="AF9" s="242"/>
+      <c r="AG9" s="242"/>
+      <c r="AH9" s="242"/>
+      <c r="AI9" s="243"/>
+      <c r="AJ9" s="241">
         <f>AJ10</f>
         <v>45061</v>
       </c>
-      <c r="AK9" s="237"/>
-      <c r="AL9" s="237"/>
-      <c r="AM9" s="237"/>
-      <c r="AN9" s="237"/>
-      <c r="AO9" s="237"/>
-      <c r="AP9" s="238"/>
-      <c r="AQ9" s="236">
+      <c r="AK9" s="242"/>
+      <c r="AL9" s="242"/>
+      <c r="AM9" s="242"/>
+      <c r="AN9" s="242"/>
+      <c r="AO9" s="242"/>
+      <c r="AP9" s="243"/>
+      <c r="AQ9" s="241">
         <f>AQ10</f>
         <v>45068</v>
       </c>
-      <c r="AR9" s="237"/>
-      <c r="AS9" s="237"/>
-      <c r="AT9" s="237"/>
-      <c r="AU9" s="237"/>
-      <c r="AV9" s="237"/>
-      <c r="AW9" s="238"/>
-      <c r="AX9" s="236">
+      <c r="AR9" s="242"/>
+      <c r="AS9" s="242"/>
+      <c r="AT9" s="242"/>
+      <c r="AU9" s="242"/>
+      <c r="AV9" s="242"/>
+      <c r="AW9" s="243"/>
+      <c r="AX9" s="241">
         <f>AX10</f>
         <v>45075</v>
       </c>
-      <c r="AY9" s="237"/>
-      <c r="AZ9" s="237"/>
-      <c r="BA9" s="237"/>
-      <c r="BB9" s="237"/>
-      <c r="BC9" s="237"/>
-      <c r="BD9" s="238"/>
-      <c r="BE9" s="236">
+      <c r="AY9" s="242"/>
+      <c r="AZ9" s="242"/>
+      <c r="BA9" s="242"/>
+      <c r="BB9" s="242"/>
+      <c r="BC9" s="242"/>
+      <c r="BD9" s="243"/>
+      <c r="BE9" s="241">
         <f>BE10</f>
         <v>45082</v>
       </c>
-      <c r="BF9" s="237"/>
-      <c r="BG9" s="237"/>
-      <c r="BH9" s="237"/>
-      <c r="BI9" s="237"/>
-      <c r="BJ9" s="237"/>
-      <c r="BK9" s="238"/>
-      <c r="BL9" s="236">
+      <c r="BF9" s="242"/>
+      <c r="BG9" s="242"/>
+      <c r="BH9" s="242"/>
+      <c r="BI9" s="242"/>
+      <c r="BJ9" s="242"/>
+      <c r="BK9" s="243"/>
+      <c r="BL9" s="241">
         <f>BL10</f>
         <v>45089</v>
       </c>
-      <c r="BM9" s="237"/>
-      <c r="BN9" s="237"/>
-      <c r="BO9" s="237"/>
-      <c r="BP9" s="237"/>
-      <c r="BQ9" s="237"/>
-      <c r="BR9" s="239"/>
+      <c r="BM9" s="242"/>
+      <c r="BN9" s="242"/>
+      <c r="BO9" s="242"/>
+      <c r="BP9" s="242"/>
+      <c r="BQ9" s="242"/>
+      <c r="BR9" s="244"/>
     </row>
     <row r="10" spans="1:70">
       <c r="O10" s="33">
@@ -17015,7 +17015,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="59" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="G13" s="142" t="s">
         <v>35</v>
@@ -17985,7 +17985,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="59" t="s">
-        <v>1148</v>
+        <v>1170</v>
       </c>
       <c r="G23" s="142" t="s">
         <v>35</v>
@@ -18082,7 +18082,7 @@
         <v>3</v>
       </c>
       <c r="F24" s="59" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="G24" s="143" t="s">
         <v>35</v>
@@ -18179,7 +18179,7 @@
         <v>4</v>
       </c>
       <c r="F25" s="59" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G25" s="142" t="s">
         <v>35</v>
@@ -18276,7 +18276,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="59" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G26" s="142" t="s">
         <v>35</v>
@@ -18373,7 +18373,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="59" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G27" s="142" t="s">
         <v>35</v>
@@ -18850,7 +18850,7 @@
         <v>3</v>
       </c>
       <c r="F32" s="59" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="G32" s="142" t="s">
         <v>35</v>
@@ -19820,7 +19820,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="59" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G42" s="142" t="s">
         <v>35</v>
@@ -19917,7 +19917,7 @@
         <v>2</v>
       </c>
       <c r="F43" s="59" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G43" s="142" t="s">
         <v>35</v>
@@ -20014,7 +20014,7 @@
         <v>3</v>
       </c>
       <c r="F44" s="59" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G44" s="142" t="s">
         <v>35</v>
@@ -20111,7 +20111,7 @@
         <v>4</v>
       </c>
       <c r="F45" s="59" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="G45" s="142" t="s">
         <v>35</v>
@@ -20297,7 +20297,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="59" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="G47" s="142" t="s">
         <v>35</v>
@@ -20394,7 +20394,7 @@
         <v>2</v>
       </c>
       <c r="F48" s="59" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="G48" s="142" t="s">
         <v>35</v>
@@ -20491,7 +20491,7 @@
         <v>3</v>
       </c>
       <c r="F49" s="59" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="G49" s="142" t="s">
         <v>35</v>
@@ -20588,7 +20588,7 @@
         <v>4</v>
       </c>
       <c r="F50" s="59" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="G50" s="142" t="s">
         <v>35</v>
@@ -20685,7 +20685,7 @@
         <v>5</v>
       </c>
       <c r="F51" s="59" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="G51" s="142" t="s">
         <v>35</v>
@@ -20871,7 +20871,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="51" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="G53" s="144" t="s">
         <v>35</v>
@@ -20968,7 +20968,7 @@
         <v>2</v>
       </c>
       <c r="F54" s="59" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="G54" s="142" t="s">
         <v>35</v>
@@ -21065,7 +21065,7 @@
         <v>3</v>
       </c>
       <c r="F55" s="59" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="G55" s="142" t="s">
         <v>35</v>
@@ -21162,7 +21162,7 @@
         <v>4</v>
       </c>
       <c r="F56" s="59" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="G56" s="142" t="s">
         <v>35</v>
@@ -21259,7 +21259,7 @@
         <v>1</v>
       </c>
       <c r="F57" s="59" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="G57" s="142" t="s">
         <v>35</v>
@@ -21356,7 +21356,7 @@
         <v>2</v>
       </c>
       <c r="F58" s="59" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="G58" s="142" t="s">
         <v>35</v>
@@ -21453,7 +21453,7 @@
         <v>3</v>
       </c>
       <c r="F59" s="59" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="G59" s="142" t="s">
         <v>35</v>
@@ -21608,12 +21608,6 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <autoFilter ref="A11:M59" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="22">
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="O8:U8"/>
-    <mergeCell ref="V8:AB8"/>
-    <mergeCell ref="AC8:AI8"/>
-    <mergeCell ref="AJ8:AP8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="A1:BR1"/>
     <mergeCell ref="A2:BR2"/>
     <mergeCell ref="A3:BR3"/>
@@ -21630,6 +21624,12 @@
     <mergeCell ref="AC9:AI9"/>
     <mergeCell ref="AJ9:AP9"/>
     <mergeCell ref="AQ9:AW9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="O8:U8"/>
+    <mergeCell ref="V8:AB8"/>
+    <mergeCell ref="AC8:AI8"/>
+    <mergeCell ref="AJ8:AP8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="L21:L22">
     <cfRule type="dataBar" priority="116">
@@ -21828,6 +21828,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
+    <cfRule type="dataBar" priority="71">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7F051754-87B9-4C18-8CD8-67421E498E01}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
     <cfRule type="dataBar" priority="79">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -21837,18 +21849,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{359FC257-C3D3-4BC8-9B18-A41F35E86C6A}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="dataBar" priority="71">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{7F051754-87B9-4C18-8CD8-67421E498E01}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -21960,11 +21960,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12:BR59">
-    <cfRule type="expression" dxfId="1" priority="327">
+    <cfRule type="expression" dxfId="1" priority="326">
+      <formula>AND($I12&lt;=O$10,ROUNDDOWN(($J12-$I12+1)*$L12,0)+$I12-1&gt;=O$10)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="327">
       <formula>AND(NOT(ISBLANK($I12)),$I12&lt;=O$10,$J12&gt;=O$10)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="326">
-      <formula>AND($I12&lt;=O$10,ROUNDDOWN(($J12-$I12+1)*$L12,0)+$I12-1&gt;=O$10)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" xWindow="1128" yWindow="374" count="1">
@@ -22220,7 +22220,7 @@
           <xm:sqref>L50 L47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{359FC257-C3D3-4BC8-9B18-A41F35E86C6A}">
+          <x14:cfRule type="dataBar" id="{7F051754-87B9-4C18-8CD8-67421E498E01}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -22232,7 +22232,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{7F051754-87B9-4C18-8CD8-67421E498E01}">
+          <x14:cfRule type="dataBar" id="{359FC257-C3D3-4BC8-9B18-A41F35E86C6A}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
@@ -22368,59 +22368,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="231"/>
-      <c r="B1" s="231"/>
-      <c r="C1" s="231"/>
-      <c r="D1" s="231"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="231"/>
-      <c r="G1" s="231"/>
-      <c r="H1" s="231"/>
-      <c r="I1" s="231"/>
-      <c r="J1" s="231"/>
-      <c r="K1" s="231"/>
-      <c r="L1" s="231"/>
-      <c r="M1" s="231"/>
+      <c r="A1" s="236"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
+      <c r="K1" s="236"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
     </row>
     <row r="2" spans="1:16" s="46" customFormat="1" ht="20.25">
-      <c r="A2" s="232" t="s">
+      <c r="A2" s="237" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="232"/>
-      <c r="C2" s="232"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
-      <c r="G2" s="232"/>
-      <c r="H2" s="232"/>
-      <c r="I2" s="232"/>
-      <c r="J2" s="232"/>
-      <c r="K2" s="232"/>
-      <c r="L2" s="232"/>
-      <c r="M2" s="232"/>
-      <c r="N2" s="232"/>
-      <c r="O2" s="232"/>
-      <c r="P2" s="232"/>
+      <c r="B2" s="237"/>
+      <c r="C2" s="237"/>
+      <c r="D2" s="237"/>
+      <c r="E2" s="237"/>
+      <c r="F2" s="237"/>
+      <c r="G2" s="237"/>
+      <c r="H2" s="237"/>
+      <c r="I2" s="237"/>
+      <c r="J2" s="237"/>
+      <c r="K2" s="237"/>
+      <c r="L2" s="237"/>
+      <c r="M2" s="237"/>
+      <c r="N2" s="237"/>
+      <c r="O2" s="237"/>
+      <c r="P2" s="237"/>
     </row>
     <row r="3" spans="1:16" s="46" customFormat="1" ht="20.25">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="237" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="232"/>
-      <c r="C3" s="232"/>
-      <c r="D3" s="232"/>
-      <c r="E3" s="232"/>
-      <c r="F3" s="232"/>
-      <c r="G3" s="232"/>
-      <c r="H3" s="232"/>
-      <c r="I3" s="232"/>
-      <c r="J3" s="232"/>
-      <c r="K3" s="232"/>
-      <c r="L3" s="232"/>
-      <c r="M3" s="232"/>
-      <c r="N3" s="232"/>
-      <c r="O3" s="232"/>
-      <c r="P3" s="232"/>
+      <c r="B3" s="237"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="237"/>
+      <c r="I3" s="237"/>
+      <c r="J3" s="237"/>
+      <c r="K3" s="237"/>
+      <c r="L3" s="237"/>
+      <c r="M3" s="237"/>
+      <c r="N3" s="237"/>
+      <c r="O3" s="237"/>
+      <c r="P3" s="237"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="67"/>
@@ -22468,59 +22468,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="231"/>
-      <c r="B1" s="231"/>
-      <c r="C1" s="231"/>
-      <c r="D1" s="231"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="231"/>
-      <c r="G1" s="231"/>
-      <c r="H1" s="231"/>
-      <c r="I1" s="231"/>
-      <c r="J1" s="231"/>
-      <c r="K1" s="231"/>
-      <c r="L1" s="231"/>
-      <c r="M1" s="231"/>
+      <c r="A1" s="236"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
+      <c r="K1" s="236"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
     </row>
     <row r="2" spans="1:16" s="46" customFormat="1" ht="20.25">
-      <c r="A2" s="232" t="s">
+      <c r="A2" s="237" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="232"/>
-      <c r="C2" s="232"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
-      <c r="G2" s="232"/>
-      <c r="H2" s="232"/>
-      <c r="I2" s="232"/>
-      <c r="J2" s="232"/>
-      <c r="K2" s="232"/>
-      <c r="L2" s="232"/>
-      <c r="M2" s="232"/>
-      <c r="N2" s="232"/>
-      <c r="O2" s="232"/>
-      <c r="P2" s="232"/>
+      <c r="B2" s="237"/>
+      <c r="C2" s="237"/>
+      <c r="D2" s="237"/>
+      <c r="E2" s="237"/>
+      <c r="F2" s="237"/>
+      <c r="G2" s="237"/>
+      <c r="H2" s="237"/>
+      <c r="I2" s="237"/>
+      <c r="J2" s="237"/>
+      <c r="K2" s="237"/>
+      <c r="L2" s="237"/>
+      <c r="M2" s="237"/>
+      <c r="N2" s="237"/>
+      <c r="O2" s="237"/>
+      <c r="P2" s="237"/>
     </row>
     <row r="3" spans="1:16" s="46" customFormat="1" ht="20.25">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="237" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="232"/>
-      <c r="C3" s="232"/>
-      <c r="D3" s="232"/>
-      <c r="E3" s="232"/>
-      <c r="F3" s="232"/>
-      <c r="G3" s="232"/>
-      <c r="H3" s="232"/>
-      <c r="I3" s="232"/>
-      <c r="J3" s="232"/>
-      <c r="K3" s="232"/>
-      <c r="L3" s="232"/>
-      <c r="M3" s="232"/>
-      <c r="N3" s="232"/>
-      <c r="O3" s="232"/>
-      <c r="P3" s="232"/>
+      <c r="B3" s="237"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="237"/>
+      <c r="I3" s="237"/>
+      <c r="J3" s="237"/>
+      <c r="K3" s="237"/>
+      <c r="L3" s="237"/>
+      <c r="M3" s="237"/>
+      <c r="N3" s="237"/>
+      <c r="O3" s="237"/>
+      <c r="P3" s="237"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="67"/>
@@ -22568,59 +22568,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="231"/>
-      <c r="B1" s="231"/>
-      <c r="C1" s="231"/>
-      <c r="D1" s="231"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="231"/>
-      <c r="G1" s="231"/>
-      <c r="H1" s="231"/>
-      <c r="I1" s="231"/>
-      <c r="J1" s="231"/>
-      <c r="K1" s="231"/>
-      <c r="L1" s="231"/>
-      <c r="M1" s="231"/>
+      <c r="A1" s="236"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
+      <c r="K1" s="236"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
     </row>
     <row r="2" spans="1:16" s="46" customFormat="1" ht="20.25">
-      <c r="A2" s="232" t="s">
+      <c r="A2" s="237" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="232"/>
-      <c r="C2" s="232"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
-      <c r="G2" s="232"/>
-      <c r="H2" s="232"/>
-      <c r="I2" s="232"/>
-      <c r="J2" s="232"/>
-      <c r="K2" s="232"/>
-      <c r="L2" s="232"/>
-      <c r="M2" s="232"/>
-      <c r="N2" s="232"/>
-      <c r="O2" s="232"/>
-      <c r="P2" s="232"/>
+      <c r="B2" s="237"/>
+      <c r="C2" s="237"/>
+      <c r="D2" s="237"/>
+      <c r="E2" s="237"/>
+      <c r="F2" s="237"/>
+      <c r="G2" s="237"/>
+      <c r="H2" s="237"/>
+      <c r="I2" s="237"/>
+      <c r="J2" s="237"/>
+      <c r="K2" s="237"/>
+      <c r="L2" s="237"/>
+      <c r="M2" s="237"/>
+      <c r="N2" s="237"/>
+      <c r="O2" s="237"/>
+      <c r="P2" s="237"/>
     </row>
     <row r="3" spans="1:16" s="46" customFormat="1" ht="20.25">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="237" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="232"/>
-      <c r="C3" s="232"/>
-      <c r="D3" s="232"/>
-      <c r="E3" s="232"/>
-      <c r="F3" s="232"/>
-      <c r="G3" s="232"/>
-      <c r="H3" s="232"/>
-      <c r="I3" s="232"/>
-      <c r="J3" s="232"/>
-      <c r="K3" s="232"/>
-      <c r="L3" s="232"/>
-      <c r="M3" s="232"/>
-      <c r="N3" s="232"/>
-      <c r="O3" s="232"/>
-      <c r="P3" s="232"/>
+      <c r="B3" s="237"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="237"/>
+      <c r="I3" s="237"/>
+      <c r="J3" s="237"/>
+      <c r="K3" s="237"/>
+      <c r="L3" s="237"/>
+      <c r="M3" s="237"/>
+      <c r="N3" s="237"/>
+      <c r="O3" s="237"/>
+      <c r="P3" s="237"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="67"/>
@@ -22668,59 +22668,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="5.0999999999999996" customHeight="1">
-      <c r="A1" s="231"/>
-      <c r="B1" s="231"/>
-      <c r="C1" s="231"/>
-      <c r="D1" s="231"/>
-      <c r="E1" s="231"/>
-      <c r="F1" s="231"/>
-      <c r="G1" s="231"/>
-      <c r="H1" s="231"/>
-      <c r="I1" s="231"/>
-      <c r="J1" s="231"/>
-      <c r="K1" s="231"/>
-      <c r="L1" s="231"/>
-      <c r="M1" s="231"/>
+      <c r="A1" s="236"/>
+      <c r="B1" s="236"/>
+      <c r="C1" s="236"/>
+      <c r="D1" s="236"/>
+      <c r="E1" s="236"/>
+      <c r="F1" s="236"/>
+      <c r="G1" s="236"/>
+      <c r="H1" s="236"/>
+      <c r="I1" s="236"/>
+      <c r="J1" s="236"/>
+      <c r="K1" s="236"/>
+      <c r="L1" s="236"/>
+      <c r="M1" s="236"/>
     </row>
     <row r="2" spans="1:16" s="46" customFormat="1" ht="20.25">
-      <c r="A2" s="232" t="s">
+      <c r="A2" s="237" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="232"/>
-      <c r="C2" s="232"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
-      <c r="G2" s="232"/>
-      <c r="H2" s="232"/>
-      <c r="I2" s="232"/>
-      <c r="J2" s="232"/>
-      <c r="K2" s="232"/>
-      <c r="L2" s="232"/>
-      <c r="M2" s="232"/>
-      <c r="N2" s="232"/>
-      <c r="O2" s="232"/>
-      <c r="P2" s="232"/>
+      <c r="B2" s="237"/>
+      <c r="C2" s="237"/>
+      <c r="D2" s="237"/>
+      <c r="E2" s="237"/>
+      <c r="F2" s="237"/>
+      <c r="G2" s="237"/>
+      <c r="H2" s="237"/>
+      <c r="I2" s="237"/>
+      <c r="J2" s="237"/>
+      <c r="K2" s="237"/>
+      <c r="L2" s="237"/>
+      <c r="M2" s="237"/>
+      <c r="N2" s="237"/>
+      <c r="O2" s="237"/>
+      <c r="P2" s="237"/>
     </row>
     <row r="3" spans="1:16" s="46" customFormat="1" ht="20.25">
-      <c r="A3" s="232" t="s">
+      <c r="A3" s="237" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="232"/>
-      <c r="C3" s="232"/>
-      <c r="D3" s="232"/>
-      <c r="E3" s="232"/>
-      <c r="F3" s="232"/>
-      <c r="G3" s="232"/>
-      <c r="H3" s="232"/>
-      <c r="I3" s="232"/>
-      <c r="J3" s="232"/>
-      <c r="K3" s="232"/>
-      <c r="L3" s="232"/>
-      <c r="M3" s="232"/>
-      <c r="N3" s="232"/>
-      <c r="O3" s="232"/>
-      <c r="P3" s="232"/>
+      <c r="B3" s="237"/>
+      <c r="C3" s="237"/>
+      <c r="D3" s="237"/>
+      <c r="E3" s="237"/>
+      <c r="F3" s="237"/>
+      <c r="G3" s="237"/>
+      <c r="H3" s="237"/>
+      <c r="I3" s="237"/>
+      <c r="J3" s="237"/>
+      <c r="K3" s="237"/>
+      <c r="L3" s="237"/>
+      <c r="M3" s="237"/>
+      <c r="N3" s="237"/>
+      <c r="O3" s="237"/>
+      <c r="P3" s="237"/>
     </row>
     <row r="4" spans="1:16" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A4" s="67"/>

</xml_diff>